<commit_message>
Refatoração dos testes dos métodos do funcionários e das mercadorias e adição dos requisitos de gerar relatório de clientes, funcionários e mercadorias.
</commit_message>
<xml_diff>
--- a/Documentacao/REQUISITOS.xlsx
+++ b/Documentacao/REQUISITOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusle\OneDrive\Documentos\CentralLojas\Projeto_Central_Lojas\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B516F76-5656-48AB-B824-35BDE6E6C5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98696A29-DE7A-41E8-8DDC-682DD6DB6E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -193,9 +193,6 @@
     <t>RD004</t>
   </si>
   <si>
-    <t>Gerar relatório diário de vendas</t>
-  </si>
-  <si>
     <t>O tempo de resposta para gerar o relatório diário deve ser inferior a 30 segundos</t>
   </si>
   <si>
@@ -230,13 +227,37 @@
   </si>
   <si>
     <t>RNF001, RD002,  RD003, RD004</t>
+  </si>
+  <si>
+    <t>Gerar relatório de vendas</t>
+  </si>
+  <si>
+    <t>RF019</t>
+  </si>
+  <si>
+    <t>Gerar relatório de clientes</t>
+  </si>
+  <si>
+    <t>Gerar relatório de funcionários</t>
+  </si>
+  <si>
+    <t>RF020</t>
+  </si>
+  <si>
+    <t>RF021</t>
+  </si>
+  <si>
+    <t>Gerar relatório de mercadorias</t>
+  </si>
+  <si>
+    <t>RNF001, RNF003, RD001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,8 +278,21 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,12 +321,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC65911"/>
         <bgColor rgb="FFC65911"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFFCE4D6"/>
       </patternFill>
     </fill>
     <fill>
@@ -355,13 +383,13 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -372,16 +400,14 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,16 +422,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -697,7 +725,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -711,7 +739,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
@@ -725,7 +753,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -739,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -753,8 +781,9 @@
         <v>16</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>62</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -767,7 +796,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
@@ -781,7 +810,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -809,7 +838,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -823,7 +852,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
@@ -837,7 +866,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -851,21 +880,21 @@
         <v>6</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="20" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -879,7 +908,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
@@ -893,7 +922,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -907,136 +936,170 @@
         <v>16</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>45</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
+      <c r="A20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="13"/>
+      <c r="A21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="12"/>
+      <c r="A34" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="12"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="12"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+    </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2004,8 +2067,9 @@
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>